<commit_message>
Suxarevskaya data with new timestamp
</commit_message>
<xml_diff>
--- a/data/Web_MEM_Suxarevskaya/2024_04_mem_suxarevskaya.xlsx
+++ b/data/Web_MEM_Suxarevskaya/2024_04_mem_suxarevskaya.xlsx
@@ -1581,7 +1581,7 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2">
-        <v>1713160800</v>
+        <v>1713150000</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -1601,7 +1601,7 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3">
-        <v>1713164400</v>
+        <v>1713153600</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
@@ -1621,7 +1621,7 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4">
-        <v>1713168000</v>
+        <v>1713157200</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
@@ -1641,7 +1641,7 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5">
-        <v>1713171600</v>
+        <v>1713160800</v>
       </c>
       <c r="B5" t="s">
         <v>14</v>
@@ -1661,7 +1661,7 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6">
-        <v>1713175200</v>
+        <v>1713164400</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
@@ -1681,7 +1681,7 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7">
-        <v>1713178800</v>
+        <v>1713168000</v>
       </c>
       <c r="B7" t="s">
         <v>16</v>
@@ -1701,7 +1701,7 @@
     </row>
     <row r="8" spans="1:11">
       <c r="A8">
-        <v>1713182400</v>
+        <v>1713171600</v>
       </c>
       <c r="B8" t="s">
         <v>17</v>
@@ -1721,7 +1721,7 @@
     </row>
     <row r="9" spans="1:11">
       <c r="A9">
-        <v>1713186000</v>
+        <v>1713175200</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
@@ -1741,7 +1741,7 @@
     </row>
     <row r="10" spans="1:11">
       <c r="A10">
-        <v>1713189600</v>
+        <v>1713178800</v>
       </c>
       <c r="B10" t="s">
         <v>19</v>
@@ -1761,7 +1761,7 @@
     </row>
     <row r="11" spans="1:11">
       <c r="A11">
-        <v>1713193200</v>
+        <v>1713182400</v>
       </c>
       <c r="B11" t="s">
         <v>20</v>
@@ -1781,7 +1781,7 @@
     </row>
     <row r="12" spans="1:11">
       <c r="A12">
-        <v>1713196800</v>
+        <v>1713186000</v>
       </c>
       <c r="B12" t="s">
         <v>21</v>
@@ -1801,7 +1801,7 @@
     </row>
     <row r="13" spans="1:11">
       <c r="A13">
-        <v>1713200400</v>
+        <v>1713189600</v>
       </c>
       <c r="B13" t="s">
         <v>22</v>
@@ -1821,7 +1821,7 @@
     </row>
     <row r="14" spans="1:11">
       <c r="A14">
-        <v>1713204000</v>
+        <v>1713193200</v>
       </c>
       <c r="B14" t="s">
         <v>23</v>
@@ -1841,7 +1841,7 @@
     </row>
     <row r="15" spans="1:11">
       <c r="A15">
-        <v>1713207600</v>
+        <v>1713196800</v>
       </c>
       <c r="B15" t="s">
         <v>24</v>
@@ -1861,7 +1861,7 @@
     </row>
     <row r="16" spans="1:11">
       <c r="A16">
-        <v>1713211200</v>
+        <v>1713200400</v>
       </c>
       <c r="B16" t="s">
         <v>25</v>
@@ -1881,7 +1881,7 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17">
-        <v>1713214800</v>
+        <v>1713204000</v>
       </c>
       <c r="B17" t="s">
         <v>26</v>
@@ -1901,7 +1901,7 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18">
-        <v>1713218400</v>
+        <v>1713207600</v>
       </c>
       <c r="B18" t="s">
         <v>27</v>
@@ -1921,7 +1921,7 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19">
-        <v>1713222000</v>
+        <v>1713211200</v>
       </c>
       <c r="B19" t="s">
         <v>28</v>
@@ -1941,7 +1941,7 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20">
-        <v>1713225600</v>
+        <v>1713214800</v>
       </c>
       <c r="B20" t="s">
         <v>29</v>
@@ -1961,7 +1961,7 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21">
-        <v>1713229200</v>
+        <v>1713218400</v>
       </c>
       <c r="B21" t="s">
         <v>30</v>
@@ -1981,7 +1981,7 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22">
-        <v>1713232800</v>
+        <v>1713222000</v>
       </c>
       <c r="B22" t="s">
         <v>31</v>
@@ -2001,7 +2001,7 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23">
-        <v>1713236400</v>
+        <v>1713225600</v>
       </c>
       <c r="B23" t="s">
         <v>32</v>
@@ -2021,7 +2021,7 @@
     </row>
     <row r="24" spans="1:8">
       <c r="A24">
-        <v>1713240000</v>
+        <v>1713229200</v>
       </c>
       <c r="B24" t="s">
         <v>33</v>
@@ -2041,7 +2041,7 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25">
-        <v>1713243600</v>
+        <v>1713232800</v>
       </c>
       <c r="B25" t="s">
         <v>34</v>
@@ -2061,7 +2061,7 @@
     </row>
     <row r="26" spans="1:8">
       <c r="A26">
-        <v>1713247200</v>
+        <v>1713236400</v>
       </c>
       <c r="B26" t="s">
         <v>35</v>
@@ -2081,7 +2081,7 @@
     </row>
     <row r="27" spans="1:8">
       <c r="A27">
-        <v>1713250800</v>
+        <v>1713240000</v>
       </c>
       <c r="B27" t="s">
         <v>36</v>
@@ -2101,7 +2101,7 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28">
-        <v>1713254400</v>
+        <v>1713243600</v>
       </c>
       <c r="B28" t="s">
         <v>37</v>
@@ -2121,7 +2121,7 @@
     </row>
     <row r="29" spans="1:8">
       <c r="A29">
-        <v>1713258000</v>
+        <v>1713247200</v>
       </c>
       <c r="B29" t="s">
         <v>38</v>
@@ -2141,7 +2141,7 @@
     </row>
     <row r="30" spans="1:8">
       <c r="A30">
-        <v>1713261600</v>
+        <v>1713250800</v>
       </c>
       <c r="B30" t="s">
         <v>39</v>
@@ -2161,7 +2161,7 @@
     </row>
     <row r="31" spans="1:8">
       <c r="A31">
-        <v>1713265200</v>
+        <v>1713254400</v>
       </c>
       <c r="B31" t="s">
         <v>40</v>
@@ -2181,7 +2181,7 @@
     </row>
     <row r="32" spans="1:8">
       <c r="A32">
-        <v>1713268800</v>
+        <v>1713258000</v>
       </c>
       <c r="B32" t="s">
         <v>41</v>
@@ -2201,7 +2201,7 @@
     </row>
     <row r="33" spans="1:8">
       <c r="A33">
-        <v>1713272400</v>
+        <v>1713261600</v>
       </c>
       <c r="B33" t="s">
         <v>42</v>
@@ -2221,7 +2221,7 @@
     </row>
     <row r="34" spans="1:8">
       <c r="A34">
-        <v>1713276000</v>
+        <v>1713265200</v>
       </c>
       <c r="B34" t="s">
         <v>43</v>
@@ -2241,7 +2241,7 @@
     </row>
     <row r="35" spans="1:8">
       <c r="A35">
-        <v>1713279600</v>
+        <v>1713268800</v>
       </c>
       <c r="B35" t="s">
         <v>44</v>
@@ -2261,7 +2261,7 @@
     </row>
     <row r="36" spans="1:8">
       <c r="A36">
-        <v>1713283200</v>
+        <v>1713272400</v>
       </c>
       <c r="B36" t="s">
         <v>45</v>
@@ -2281,7 +2281,7 @@
     </row>
     <row r="37" spans="1:8">
       <c r="A37">
-        <v>1713286800</v>
+        <v>1713276000</v>
       </c>
       <c r="B37" t="s">
         <v>46</v>
@@ -2301,7 +2301,7 @@
     </row>
     <row r="38" spans="1:8">
       <c r="A38">
-        <v>1713290400</v>
+        <v>1713279600</v>
       </c>
       <c r="B38" t="s">
         <v>47</v>
@@ -2321,7 +2321,7 @@
     </row>
     <row r="39" spans="1:8">
       <c r="A39">
-        <v>1713294000</v>
+        <v>1713283200</v>
       </c>
       <c r="B39" t="s">
         <v>48</v>
@@ -2341,7 +2341,7 @@
     </row>
     <row r="40" spans="1:8">
       <c r="A40">
-        <v>1713297600</v>
+        <v>1713286800</v>
       </c>
       <c r="B40" t="s">
         <v>49</v>
@@ -2361,7 +2361,7 @@
     </row>
     <row r="41" spans="1:8">
       <c r="A41">
-        <v>1713301200</v>
+        <v>1713290400</v>
       </c>
       <c r="B41" t="s">
         <v>50</v>
@@ -2381,7 +2381,7 @@
     </row>
     <row r="42" spans="1:8">
       <c r="A42">
-        <v>1713304800</v>
+        <v>1713294000</v>
       </c>
       <c r="B42" t="s">
         <v>51</v>
@@ -2401,7 +2401,7 @@
     </row>
     <row r="43" spans="1:8">
       <c r="A43">
-        <v>1713308400</v>
+        <v>1713297600</v>
       </c>
       <c r="B43" t="s">
         <v>52</v>
@@ -2421,7 +2421,7 @@
     </row>
     <row r="44" spans="1:8">
       <c r="A44">
-        <v>1713312000</v>
+        <v>1713301200</v>
       </c>
       <c r="B44" t="s">
         <v>53</v>
@@ -2441,7 +2441,7 @@
     </row>
     <row r="45" spans="1:8">
       <c r="A45">
-        <v>1713315600</v>
+        <v>1713304800</v>
       </c>
       <c r="B45" t="s">
         <v>54</v>
@@ -2461,7 +2461,7 @@
     </row>
     <row r="46" spans="1:8">
       <c r="A46">
-        <v>1713319200</v>
+        <v>1713308400</v>
       </c>
       <c r="B46" t="s">
         <v>55</v>
@@ -2481,7 +2481,7 @@
     </row>
     <row r="47" spans="1:8">
       <c r="A47">
-        <v>1713322800</v>
+        <v>1713312000</v>
       </c>
       <c r="B47" t="s">
         <v>56</v>
@@ -2501,7 +2501,7 @@
     </row>
     <row r="48" spans="1:8">
       <c r="A48">
-        <v>1713326400</v>
+        <v>1713315600</v>
       </c>
       <c r="B48" t="s">
         <v>57</v>
@@ -2521,7 +2521,7 @@
     </row>
     <row r="49" spans="1:8">
       <c r="A49">
-        <v>1713330000</v>
+        <v>1713319200</v>
       </c>
       <c r="B49" t="s">
         <v>58</v>
@@ -2541,7 +2541,7 @@
     </row>
     <row r="50" spans="1:8">
       <c r="A50">
-        <v>1713333600</v>
+        <v>1713322800</v>
       </c>
       <c r="B50" t="s">
         <v>59</v>
@@ -2561,7 +2561,7 @@
     </row>
     <row r="51" spans="1:8">
       <c r="A51">
-        <v>1713337200</v>
+        <v>1713326400</v>
       </c>
       <c r="B51" t="s">
         <v>60</v>
@@ -2581,7 +2581,7 @@
     </row>
     <row r="52" spans="1:8">
       <c r="A52">
-        <v>1713340800</v>
+        <v>1713330000</v>
       </c>
       <c r="B52" t="s">
         <v>61</v>
@@ -2601,7 +2601,7 @@
     </row>
     <row r="53" spans="1:8">
       <c r="A53">
-        <v>1713344400</v>
+        <v>1713333600</v>
       </c>
       <c r="B53" t="s">
         <v>62</v>
@@ -2621,7 +2621,7 @@
     </row>
     <row r="54" spans="1:8">
       <c r="A54">
-        <v>1713348000</v>
+        <v>1713337200</v>
       </c>
       <c r="B54" t="s">
         <v>63</v>
@@ -2641,7 +2641,7 @@
     </row>
     <row r="55" spans="1:8">
       <c r="A55">
-        <v>1713351600</v>
+        <v>1713340800</v>
       </c>
       <c r="B55" t="s">
         <v>64</v>
@@ -2661,7 +2661,7 @@
     </row>
     <row r="56" spans="1:8">
       <c r="A56">
-        <v>1713355200</v>
+        <v>1713344400</v>
       </c>
       <c r="B56" t="s">
         <v>65</v>
@@ -2681,7 +2681,7 @@
     </row>
     <row r="57" spans="1:8">
       <c r="A57">
-        <v>1713358800</v>
+        <v>1713348000</v>
       </c>
       <c r="B57" t="s">
         <v>66</v>
@@ -2701,7 +2701,7 @@
     </row>
     <row r="58" spans="1:8">
       <c r="A58">
-        <v>1713362400</v>
+        <v>1713351600</v>
       </c>
       <c r="B58" t="s">
         <v>67</v>
@@ -2721,7 +2721,7 @@
     </row>
     <row r="59" spans="1:8">
       <c r="A59">
-        <v>1713366000</v>
+        <v>1713355200</v>
       </c>
       <c r="B59" t="s">
         <v>68</v>
@@ -2741,7 +2741,7 @@
     </row>
     <row r="60" spans="1:8">
       <c r="A60">
-        <v>1713369600</v>
+        <v>1713358800</v>
       </c>
       <c r="B60" t="s">
         <v>69</v>
@@ -2761,7 +2761,7 @@
     </row>
     <row r="61" spans="1:8">
       <c r="A61">
-        <v>1713373200</v>
+        <v>1713362400</v>
       </c>
       <c r="B61" t="s">
         <v>70</v>
@@ -2781,7 +2781,7 @@
     </row>
     <row r="62" spans="1:8">
       <c r="A62">
-        <v>1713376800</v>
+        <v>1713366000</v>
       </c>
       <c r="B62" t="s">
         <v>71</v>
@@ -2801,7 +2801,7 @@
     </row>
     <row r="63" spans="1:8">
       <c r="A63">
-        <v>1713380400</v>
+        <v>1713369600</v>
       </c>
       <c r="B63" t="s">
         <v>72</v>
@@ -2821,7 +2821,7 @@
     </row>
     <row r="64" spans="1:8">
       <c r="A64">
-        <v>1713384000</v>
+        <v>1713373200</v>
       </c>
       <c r="B64" t="s">
         <v>73</v>
@@ -2841,7 +2841,7 @@
     </row>
     <row r="65" spans="1:8">
       <c r="A65">
-        <v>1713387600</v>
+        <v>1713376800</v>
       </c>
       <c r="B65" t="s">
         <v>74</v>
@@ -2861,7 +2861,7 @@
     </row>
     <row r="66" spans="1:8">
       <c r="A66">
-        <v>1713391200</v>
+        <v>1713380400</v>
       </c>
       <c r="B66" t="s">
         <v>75</v>
@@ -2881,7 +2881,7 @@
     </row>
     <row r="67" spans="1:8">
       <c r="A67">
-        <v>1713394800</v>
+        <v>1713384000</v>
       </c>
       <c r="B67" t="s">
         <v>76</v>
@@ -2901,7 +2901,7 @@
     </row>
     <row r="68" spans="1:8">
       <c r="A68">
-        <v>1713398400</v>
+        <v>1713387600</v>
       </c>
       <c r="B68" t="s">
         <v>77</v>
@@ -2921,7 +2921,7 @@
     </row>
     <row r="69" spans="1:8">
       <c r="A69">
-        <v>1713402000</v>
+        <v>1713391200</v>
       </c>
       <c r="B69" t="s">
         <v>78</v>
@@ -2941,7 +2941,7 @@
     </row>
     <row r="70" spans="1:8">
       <c r="A70">
-        <v>1713405600</v>
+        <v>1713394800</v>
       </c>
       <c r="B70" t="s">
         <v>79</v>
@@ -2961,7 +2961,7 @@
     </row>
     <row r="71" spans="1:8">
       <c r="A71">
-        <v>1713409200</v>
+        <v>1713398400</v>
       </c>
       <c r="B71" t="s">
         <v>80</v>
@@ -2981,7 +2981,7 @@
     </row>
     <row r="72" spans="1:8">
       <c r="A72">
-        <v>1713412800</v>
+        <v>1713402000</v>
       </c>
       <c r="B72" t="s">
         <v>81</v>
@@ -3001,7 +3001,7 @@
     </row>
     <row r="73" spans="1:8">
       <c r="A73">
-        <v>1713416400</v>
+        <v>1713405600</v>
       </c>
       <c r="B73" t="s">
         <v>82</v>
@@ -3021,7 +3021,7 @@
     </row>
     <row r="74" spans="1:8">
       <c r="A74">
-        <v>1713420000</v>
+        <v>1713409200</v>
       </c>
       <c r="B74" t="s">
         <v>83</v>
@@ -3041,7 +3041,7 @@
     </row>
     <row r="75" spans="1:8">
       <c r="A75">
-        <v>1713423600</v>
+        <v>1713412800</v>
       </c>
       <c r="B75" t="s">
         <v>84</v>
@@ -3061,7 +3061,7 @@
     </row>
     <row r="76" spans="1:8">
       <c r="A76">
-        <v>1713427200</v>
+        <v>1713416400</v>
       </c>
       <c r="B76" t="s">
         <v>85</v>
@@ -3081,7 +3081,7 @@
     </row>
     <row r="77" spans="1:8">
       <c r="A77">
-        <v>1713430800</v>
+        <v>1713420000</v>
       </c>
       <c r="B77" t="s">
         <v>86</v>
@@ -3101,7 +3101,7 @@
     </row>
     <row r="78" spans="1:8">
       <c r="A78">
-        <v>1713434400</v>
+        <v>1713423600</v>
       </c>
       <c r="B78" t="s">
         <v>87</v>
@@ -3121,7 +3121,7 @@
     </row>
     <row r="79" spans="1:8">
       <c r="A79">
-        <v>1713438000</v>
+        <v>1713427200</v>
       </c>
       <c r="B79" t="s">
         <v>88</v>
@@ -3141,7 +3141,7 @@
     </row>
     <row r="80" spans="1:8">
       <c r="A80">
-        <v>1713441600</v>
+        <v>1713430800</v>
       </c>
       <c r="B80" t="s">
         <v>89</v>
@@ -3161,7 +3161,7 @@
     </row>
     <row r="81" spans="1:8">
       <c r="A81">
-        <v>1713445200</v>
+        <v>1713434400</v>
       </c>
       <c r="B81" t="s">
         <v>90</v>
@@ -3181,7 +3181,7 @@
     </row>
     <row r="82" spans="1:8">
       <c r="A82">
-        <v>1713448800</v>
+        <v>1713438000</v>
       </c>
       <c r="B82" t="s">
         <v>91</v>
@@ -3201,7 +3201,7 @@
     </row>
     <row r="83" spans="1:8">
       <c r="A83">
-        <v>1713452400</v>
+        <v>1713441600</v>
       </c>
       <c r="B83" t="s">
         <v>92</v>
@@ -3221,7 +3221,7 @@
     </row>
     <row r="84" spans="1:8">
       <c r="A84">
-        <v>1713456000</v>
+        <v>1713445200</v>
       </c>
       <c r="B84" t="s">
         <v>93</v>
@@ -3241,7 +3241,7 @@
     </row>
     <row r="85" spans="1:8">
       <c r="A85">
-        <v>1713459600</v>
+        <v>1713448800</v>
       </c>
       <c r="B85" t="s">
         <v>94</v>
@@ -3261,7 +3261,7 @@
     </row>
     <row r="86" spans="1:8">
       <c r="A86">
-        <v>1713463200</v>
+        <v>1713452400</v>
       </c>
       <c r="B86" t="s">
         <v>95</v>
@@ -3281,7 +3281,7 @@
     </row>
     <row r="87" spans="1:8">
       <c r="A87">
-        <v>1713466800</v>
+        <v>1713456000</v>
       </c>
       <c r="B87" t="s">
         <v>96</v>
@@ -3301,7 +3301,7 @@
     </row>
     <row r="88" spans="1:8">
       <c r="A88">
-        <v>1713470400</v>
+        <v>1713459600</v>
       </c>
       <c r="B88" t="s">
         <v>97</v>
@@ -3321,7 +3321,7 @@
     </row>
     <row r="89" spans="1:8">
       <c r="A89">
-        <v>1713474000</v>
+        <v>1713463200</v>
       </c>
       <c r="B89" t="s">
         <v>98</v>
@@ -3341,7 +3341,7 @@
     </row>
     <row r="90" spans="1:8">
       <c r="A90">
-        <v>1713477600</v>
+        <v>1713466800</v>
       </c>
       <c r="B90" t="s">
         <v>99</v>
@@ -3361,7 +3361,7 @@
     </row>
     <row r="91" spans="1:8">
       <c r="A91">
-        <v>1713481200</v>
+        <v>1713470400</v>
       </c>
       <c r="B91" t="s">
         <v>100</v>
@@ -3381,7 +3381,7 @@
     </row>
     <row r="92" spans="1:8">
       <c r="A92">
-        <v>1713484800</v>
+        <v>1713474000</v>
       </c>
       <c r="B92" t="s">
         <v>101</v>
@@ -3401,7 +3401,7 @@
     </row>
     <row r="93" spans="1:8">
       <c r="A93">
-        <v>1713488400</v>
+        <v>1713477600</v>
       </c>
       <c r="B93" t="s">
         <v>102</v>
@@ -3421,7 +3421,7 @@
     </row>
     <row r="94" spans="1:8">
       <c r="A94">
-        <v>1713492000</v>
+        <v>1713481200</v>
       </c>
       <c r="B94" t="s">
         <v>103</v>
@@ -3441,7 +3441,7 @@
     </row>
     <row r="95" spans="1:8">
       <c r="A95">
-        <v>1713495600</v>
+        <v>1713484800</v>
       </c>
       <c r="B95" t="s">
         <v>104</v>
@@ -3461,7 +3461,7 @@
     </row>
     <row r="96" spans="1:8">
       <c r="A96">
-        <v>1713499200</v>
+        <v>1713488400</v>
       </c>
       <c r="B96" t="s">
         <v>105</v>
@@ -3481,7 +3481,7 @@
     </row>
     <row r="97" spans="1:8">
       <c r="A97">
-        <v>1713502800</v>
+        <v>1713492000</v>
       </c>
       <c r="B97" t="s">
         <v>106</v>
@@ -3501,7 +3501,7 @@
     </row>
     <row r="98" spans="1:8">
       <c r="A98">
-        <v>1713506400</v>
+        <v>1713495600</v>
       </c>
       <c r="B98" t="s">
         <v>107</v>
@@ -3521,7 +3521,7 @@
     </row>
     <row r="99" spans="1:8">
       <c r="A99">
-        <v>1713510000</v>
+        <v>1713499200</v>
       </c>
       <c r="B99" t="s">
         <v>108</v>
@@ -3541,7 +3541,7 @@
     </row>
     <row r="100" spans="1:8">
       <c r="A100">
-        <v>1713513600</v>
+        <v>1713502800</v>
       </c>
       <c r="B100" t="s">
         <v>109</v>
@@ -3561,7 +3561,7 @@
     </row>
     <row r="101" spans="1:8">
       <c r="A101">
-        <v>1713517200</v>
+        <v>1713506400</v>
       </c>
       <c r="B101" t="s">
         <v>110</v>
@@ -3581,7 +3581,7 @@
     </row>
     <row r="102" spans="1:8">
       <c r="A102">
-        <v>1713520800</v>
+        <v>1713510000</v>
       </c>
       <c r="B102" t="s">
         <v>111</v>
@@ -3601,7 +3601,7 @@
     </row>
     <row r="103" spans="1:8">
       <c r="A103">
-        <v>1713524400</v>
+        <v>1713513600</v>
       </c>
       <c r="B103" t="s">
         <v>112</v>
@@ -3621,7 +3621,7 @@
     </row>
     <row r="104" spans="1:8">
       <c r="A104">
-        <v>1713528000</v>
+        <v>1713517200</v>
       </c>
       <c r="B104" t="s">
         <v>113</v>
@@ -3641,7 +3641,7 @@
     </row>
     <row r="105" spans="1:8">
       <c r="A105">
-        <v>1713531600</v>
+        <v>1713520800</v>
       </c>
       <c r="B105" t="s">
         <v>114</v>
@@ -3661,7 +3661,7 @@
     </row>
     <row r="106" spans="1:8">
       <c r="A106">
-        <v>1713535200</v>
+        <v>1713524400</v>
       </c>
       <c r="B106" t="s">
         <v>115</v>
@@ -3681,7 +3681,7 @@
     </row>
     <row r="107" spans="1:8">
       <c r="A107">
-        <v>1713538800</v>
+        <v>1713528000</v>
       </c>
       <c r="B107" t="s">
         <v>116</v>
@@ -3701,7 +3701,7 @@
     </row>
     <row r="108" spans="1:8">
       <c r="A108">
-        <v>1713542400</v>
+        <v>1713531600</v>
       </c>
       <c r="B108" t="s">
         <v>117</v>
@@ -3721,7 +3721,7 @@
     </row>
     <row r="109" spans="1:8">
       <c r="A109">
-        <v>1713546000</v>
+        <v>1713535200</v>
       </c>
       <c r="B109" t="s">
         <v>118</v>
@@ -3741,7 +3741,7 @@
     </row>
     <row r="110" spans="1:8">
       <c r="A110">
-        <v>1713549600</v>
+        <v>1713538800</v>
       </c>
       <c r="B110" t="s">
         <v>119</v>
@@ -3761,7 +3761,7 @@
     </row>
     <row r="111" spans="1:8">
       <c r="A111">
-        <v>1713553200</v>
+        <v>1713542400</v>
       </c>
       <c r="B111" t="s">
         <v>120</v>
@@ -3781,7 +3781,7 @@
     </row>
     <row r="112" spans="1:8">
       <c r="A112">
-        <v>1713556800</v>
+        <v>1713546000</v>
       </c>
       <c r="B112" t="s">
         <v>121</v>
@@ -3801,7 +3801,7 @@
     </row>
     <row r="113" spans="1:8">
       <c r="A113">
-        <v>1713560400</v>
+        <v>1713549600</v>
       </c>
       <c r="B113" t="s">
         <v>122</v>
@@ -3821,7 +3821,7 @@
     </row>
     <row r="114" spans="1:8">
       <c r="A114">
-        <v>1713564000</v>
+        <v>1713553200</v>
       </c>
       <c r="B114" t="s">
         <v>123</v>
@@ -3841,7 +3841,7 @@
     </row>
     <row r="115" spans="1:8">
       <c r="A115">
-        <v>1713567600</v>
+        <v>1713556800</v>
       </c>
       <c r="B115" t="s">
         <v>124</v>
@@ -3861,7 +3861,7 @@
     </row>
     <row r="116" spans="1:8">
       <c r="A116">
-        <v>1713571200</v>
+        <v>1713560400</v>
       </c>
       <c r="B116" t="s">
         <v>125</v>
@@ -3881,7 +3881,7 @@
     </row>
     <row r="117" spans="1:8">
       <c r="A117">
-        <v>1713574800</v>
+        <v>1713564000</v>
       </c>
       <c r="B117" t="s">
         <v>126</v>
@@ -3901,7 +3901,7 @@
     </row>
     <row r="118" spans="1:8">
       <c r="A118">
-        <v>1713578400</v>
+        <v>1713567600</v>
       </c>
       <c r="B118" t="s">
         <v>127</v>
@@ -3921,7 +3921,7 @@
     </row>
     <row r="119" spans="1:8">
       <c r="A119">
-        <v>1713582000</v>
+        <v>1713571200</v>
       </c>
       <c r="B119" t="s">
         <v>128</v>
@@ -3941,7 +3941,7 @@
     </row>
     <row r="120" spans="1:8">
       <c r="A120">
-        <v>1713585600</v>
+        <v>1713574800</v>
       </c>
       <c r="B120" t="s">
         <v>129</v>
@@ -3961,7 +3961,7 @@
     </row>
     <row r="121" spans="1:8">
       <c r="A121">
-        <v>1713589200</v>
+        <v>1713578400</v>
       </c>
       <c r="B121" t="s">
         <v>130</v>
@@ -3981,7 +3981,7 @@
     </row>
     <row r="122" spans="1:8">
       <c r="A122">
-        <v>1713592800</v>
+        <v>1713582000</v>
       </c>
       <c r="B122" t="s">
         <v>131</v>
@@ -4001,7 +4001,7 @@
     </row>
     <row r="123" spans="1:8">
       <c r="A123">
-        <v>1713596400</v>
+        <v>1713585600</v>
       </c>
       <c r="B123" t="s">
         <v>132</v>
@@ -4021,7 +4021,7 @@
     </row>
     <row r="124" spans="1:8">
       <c r="A124">
-        <v>1713600000</v>
+        <v>1713589200</v>
       </c>
       <c r="B124" t="s">
         <v>133</v>
@@ -4041,7 +4041,7 @@
     </row>
     <row r="125" spans="1:8">
       <c r="A125">
-        <v>1713603600</v>
+        <v>1713592800</v>
       </c>
       <c r="B125" t="s">
         <v>134</v>
@@ -4061,7 +4061,7 @@
     </row>
     <row r="126" spans="1:8">
       <c r="A126">
-        <v>1713607200</v>
+        <v>1713596400</v>
       </c>
       <c r="B126" t="s">
         <v>135</v>
@@ -4081,7 +4081,7 @@
     </row>
     <row r="127" spans="1:8">
       <c r="A127">
-        <v>1713610800</v>
+        <v>1713600000</v>
       </c>
       <c r="B127" t="s">
         <v>136</v>
@@ -4101,7 +4101,7 @@
     </row>
     <row r="128" spans="1:8">
       <c r="A128">
-        <v>1713614400</v>
+        <v>1713603600</v>
       </c>
       <c r="B128" t="s">
         <v>137</v>
@@ -4121,7 +4121,7 @@
     </row>
     <row r="129" spans="1:8">
       <c r="A129">
-        <v>1713618000</v>
+        <v>1713607200</v>
       </c>
       <c r="B129" t="s">
         <v>138</v>
@@ -4141,7 +4141,7 @@
     </row>
     <row r="130" spans="1:8">
       <c r="A130">
-        <v>1713621600</v>
+        <v>1713610800</v>
       </c>
       <c r="B130" t="s">
         <v>139</v>
@@ -4161,7 +4161,7 @@
     </row>
     <row r="131" spans="1:8">
       <c r="A131">
-        <v>1713625200</v>
+        <v>1713614400</v>
       </c>
       <c r="B131" t="s">
         <v>140</v>
@@ -4181,7 +4181,7 @@
     </row>
     <row r="132" spans="1:8">
       <c r="A132">
-        <v>1713628800</v>
+        <v>1713618000</v>
       </c>
       <c r="B132" t="s">
         <v>141</v>
@@ -4201,7 +4201,7 @@
     </row>
     <row r="133" spans="1:8">
       <c r="A133">
-        <v>1713632400</v>
+        <v>1713621600</v>
       </c>
       <c r="B133" t="s">
         <v>142</v>
@@ -4221,7 +4221,7 @@
     </row>
     <row r="134" spans="1:8">
       <c r="A134">
-        <v>1713636000</v>
+        <v>1713625200</v>
       </c>
       <c r="B134" t="s">
         <v>143</v>
@@ -4241,7 +4241,7 @@
     </row>
     <row r="135" spans="1:8">
       <c r="A135">
-        <v>1713639600</v>
+        <v>1713628800</v>
       </c>
       <c r="B135" t="s">
         <v>144</v>
@@ -4261,7 +4261,7 @@
     </row>
     <row r="136" spans="1:8">
       <c r="A136">
-        <v>1713643200</v>
+        <v>1713632400</v>
       </c>
       <c r="B136" t="s">
         <v>145</v>
@@ -4281,7 +4281,7 @@
     </row>
     <row r="137" spans="1:8">
       <c r="A137">
-        <v>1713646800</v>
+        <v>1713636000</v>
       </c>
       <c r="B137" t="s">
         <v>146</v>
@@ -4301,7 +4301,7 @@
     </row>
     <row r="138" spans="1:8">
       <c r="A138">
-        <v>1713650400</v>
+        <v>1713639600</v>
       </c>
       <c r="B138" t="s">
         <v>147</v>
@@ -4321,7 +4321,7 @@
     </row>
     <row r="139" spans="1:8">
       <c r="A139">
-        <v>1713654000</v>
+        <v>1713643200</v>
       </c>
       <c r="B139" t="s">
         <v>148</v>
@@ -4341,7 +4341,7 @@
     </row>
     <row r="140" spans="1:8">
       <c r="A140">
-        <v>1713657600</v>
+        <v>1713646800</v>
       </c>
       <c r="B140" t="s">
         <v>149</v>
@@ -4361,7 +4361,7 @@
     </row>
     <row r="141" spans="1:8">
       <c r="A141">
-        <v>1713661200</v>
+        <v>1713650400</v>
       </c>
       <c r="B141" t="s">
         <v>150</v>
@@ -4381,7 +4381,7 @@
     </row>
     <row r="142" spans="1:8">
       <c r="A142">
-        <v>1713664800</v>
+        <v>1713654000</v>
       </c>
       <c r="B142" t="s">
         <v>151</v>
@@ -4401,7 +4401,7 @@
     </row>
     <row r="143" spans="1:8">
       <c r="A143">
-        <v>1713668400</v>
+        <v>1713657600</v>
       </c>
       <c r="B143" t="s">
         <v>152</v>
@@ -4421,7 +4421,7 @@
     </row>
     <row r="144" spans="1:8">
       <c r="A144">
-        <v>1713672000</v>
+        <v>1713661200</v>
       </c>
       <c r="B144" t="s">
         <v>153</v>
@@ -4441,7 +4441,7 @@
     </row>
     <row r="145" spans="1:8">
       <c r="A145">
-        <v>1713675600</v>
+        <v>1713664800</v>
       </c>
       <c r="B145" t="s">
         <v>154</v>
@@ -4461,7 +4461,7 @@
     </row>
     <row r="146" spans="1:8">
       <c r="A146">
-        <v>1713679200</v>
+        <v>1713668400</v>
       </c>
       <c r="B146" t="s">
         <v>155</v>
@@ -4481,7 +4481,7 @@
     </row>
     <row r="147" spans="1:8">
       <c r="A147">
-        <v>1713682800</v>
+        <v>1713672000</v>
       </c>
       <c r="B147" t="s">
         <v>156</v>
@@ -4501,7 +4501,7 @@
     </row>
     <row r="148" spans="1:8">
       <c r="A148">
-        <v>1713686400</v>
+        <v>1713675600</v>
       </c>
       <c r="B148" t="s">
         <v>157</v>
@@ -4521,7 +4521,7 @@
     </row>
     <row r="149" spans="1:8">
       <c r="A149">
-        <v>1713690000</v>
+        <v>1713679200</v>
       </c>
       <c r="B149" t="s">
         <v>158</v>
@@ -4541,7 +4541,7 @@
     </row>
     <row r="150" spans="1:8">
       <c r="A150">
-        <v>1713693600</v>
+        <v>1713682800</v>
       </c>
       <c r="B150" t="s">
         <v>159</v>
@@ -4561,7 +4561,7 @@
     </row>
     <row r="151" spans="1:8">
       <c r="A151">
-        <v>1713697200</v>
+        <v>1713686400</v>
       </c>
       <c r="B151" t="s">
         <v>160</v>
@@ -4581,7 +4581,7 @@
     </row>
     <row r="152" spans="1:8">
       <c r="A152">
-        <v>1713700800</v>
+        <v>1713690000</v>
       </c>
       <c r="B152" t="s">
         <v>161</v>
@@ -4601,7 +4601,7 @@
     </row>
     <row r="153" spans="1:8">
       <c r="A153">
-        <v>1713704400</v>
+        <v>1713693600</v>
       </c>
       <c r="B153" t="s">
         <v>162</v>
@@ -4621,7 +4621,7 @@
     </row>
     <row r="154" spans="1:8">
       <c r="A154">
-        <v>1713708000</v>
+        <v>1713697200</v>
       </c>
       <c r="B154" t="s">
         <v>163</v>
@@ -4641,7 +4641,7 @@
     </row>
     <row r="155" spans="1:8">
       <c r="A155">
-        <v>1713711600</v>
+        <v>1713700800</v>
       </c>
       <c r="B155" t="s">
         <v>164</v>
@@ -4661,7 +4661,7 @@
     </row>
     <row r="156" spans="1:8">
       <c r="A156">
-        <v>1713715200</v>
+        <v>1713704400</v>
       </c>
       <c r="B156" t="s">
         <v>165</v>
@@ -4681,7 +4681,7 @@
     </row>
     <row r="157" spans="1:8">
       <c r="A157">
-        <v>1713718800</v>
+        <v>1713708000</v>
       </c>
       <c r="B157" t="s">
         <v>166</v>
@@ -4701,7 +4701,7 @@
     </row>
     <row r="158" spans="1:8">
       <c r="A158">
-        <v>1713722400</v>
+        <v>1713711600</v>
       </c>
       <c r="B158" t="s">
         <v>167</v>
@@ -4721,7 +4721,7 @@
     </row>
     <row r="159" spans="1:8">
       <c r="A159">
-        <v>1713726000</v>
+        <v>1713715200</v>
       </c>
       <c r="B159" t="s">
         <v>168</v>
@@ -4741,7 +4741,7 @@
     </row>
     <row r="160" spans="1:8">
       <c r="A160">
-        <v>1713729600</v>
+        <v>1713718800</v>
       </c>
       <c r="B160" t="s">
         <v>169</v>
@@ -4761,7 +4761,7 @@
     </row>
     <row r="161" spans="1:8">
       <c r="A161">
-        <v>1713733200</v>
+        <v>1713722400</v>
       </c>
       <c r="B161" t="s">
         <v>170</v>
@@ -4781,7 +4781,7 @@
     </row>
     <row r="162" spans="1:8">
       <c r="A162">
-        <v>1713736800</v>
+        <v>1713726000</v>
       </c>
       <c r="B162" t="s">
         <v>171</v>
@@ -4801,7 +4801,7 @@
     </row>
     <row r="163" spans="1:8">
       <c r="A163">
-        <v>1713740400</v>
+        <v>1713729600</v>
       </c>
       <c r="B163" t="s">
         <v>172</v>
@@ -4821,7 +4821,7 @@
     </row>
     <row r="164" spans="1:8">
       <c r="A164">
-        <v>1713744000</v>
+        <v>1713733200</v>
       </c>
       <c r="B164" t="s">
         <v>173</v>
@@ -4841,7 +4841,7 @@
     </row>
     <row r="165" spans="1:8">
       <c r="A165">
-        <v>1713747600</v>
+        <v>1713736800</v>
       </c>
       <c r="B165" t="s">
         <v>174</v>
@@ -4861,7 +4861,7 @@
     </row>
     <row r="166" spans="1:8">
       <c r="A166">
-        <v>1713751200</v>
+        <v>1713740400</v>
       </c>
       <c r="B166" t="s">
         <v>175</v>
@@ -4881,7 +4881,7 @@
     </row>
     <row r="167" spans="1:8">
       <c r="A167">
-        <v>1713754800</v>
+        <v>1713744000</v>
       </c>
       <c r="B167" t="s">
         <v>176</v>
@@ -4901,7 +4901,7 @@
     </row>
     <row r="168" spans="1:8">
       <c r="A168">
-        <v>1713758400</v>
+        <v>1713747600</v>
       </c>
       <c r="B168" t="s">
         <v>177</v>
@@ -4921,7 +4921,7 @@
     </row>
     <row r="169" spans="1:8">
       <c r="A169">
-        <v>1713762000</v>
+        <v>1713751200</v>
       </c>
       <c r="B169" t="s">
         <v>178</v>
@@ -4941,7 +4941,7 @@
     </row>
     <row r="170" spans="1:8">
       <c r="A170">
-        <v>1713765600</v>
+        <v>1713754800</v>
       </c>
       <c r="B170" t="s">
         <v>179</v>
@@ -4961,7 +4961,7 @@
     </row>
     <row r="171" spans="1:8">
       <c r="A171">
-        <v>1713769200</v>
+        <v>1713758400</v>
       </c>
       <c r="B171" t="s">
         <v>180</v>
@@ -4981,7 +4981,7 @@
     </row>
     <row r="172" spans="1:8">
       <c r="A172">
-        <v>1713772800</v>
+        <v>1713762000</v>
       </c>
       <c r="B172" t="s">
         <v>181</v>
@@ -5001,7 +5001,7 @@
     </row>
     <row r="173" spans="1:8">
       <c r="A173">
-        <v>1713776400</v>
+        <v>1713765600</v>
       </c>
       <c r="B173" t="s">
         <v>182</v>
@@ -5021,7 +5021,7 @@
     </row>
     <row r="174" spans="1:8">
       <c r="A174">
-        <v>1713780000</v>
+        <v>1713769200</v>
       </c>
       <c r="B174" t="s">
         <v>183</v>
@@ -5041,7 +5041,7 @@
     </row>
     <row r="175" spans="1:8">
       <c r="A175">
-        <v>1713783600</v>
+        <v>1713772800</v>
       </c>
       <c r="B175" t="s">
         <v>184</v>
@@ -5061,7 +5061,7 @@
     </row>
     <row r="176" spans="1:8">
       <c r="A176">
-        <v>1713787200</v>
+        <v>1713776400</v>
       </c>
       <c r="B176" t="s">
         <v>185</v>
@@ -5081,7 +5081,7 @@
     </row>
     <row r="177" spans="1:8">
       <c r="A177">
-        <v>1713790800</v>
+        <v>1713780000</v>
       </c>
       <c r="B177" t="s">
         <v>186</v>
@@ -5101,7 +5101,7 @@
     </row>
     <row r="178" spans="1:8">
       <c r="A178">
-        <v>1713794400</v>
+        <v>1713783600</v>
       </c>
       <c r="B178" t="s">
         <v>187</v>
@@ -5121,7 +5121,7 @@
     </row>
     <row r="179" spans="1:8">
       <c r="A179">
-        <v>1713798000</v>
+        <v>1713787200</v>
       </c>
       <c r="B179" t="s">
         <v>188</v>
@@ -5141,7 +5141,7 @@
     </row>
     <row r="180" spans="1:8">
       <c r="A180">
-        <v>1713801600</v>
+        <v>1713790800</v>
       </c>
       <c r="B180" t="s">
         <v>189</v>
@@ -5161,7 +5161,7 @@
     </row>
     <row r="181" spans="1:8">
       <c r="A181">
-        <v>1713805200</v>
+        <v>1713794400</v>
       </c>
       <c r="B181" t="s">
         <v>190</v>
@@ -5181,7 +5181,7 @@
     </row>
     <row r="182" spans="1:8">
       <c r="A182">
-        <v>1713808800</v>
+        <v>1713798000</v>
       </c>
       <c r="B182" t="s">
         <v>191</v>
@@ -5201,7 +5201,7 @@
     </row>
     <row r="183" spans="1:8">
       <c r="A183">
-        <v>1713812400</v>
+        <v>1713801600</v>
       </c>
       <c r="B183" t="s">
         <v>192</v>
@@ -5221,7 +5221,7 @@
     </row>
     <row r="184" spans="1:8">
       <c r="A184">
-        <v>1713816000</v>
+        <v>1713805200</v>
       </c>
       <c r="B184" t="s">
         <v>193</v>
@@ -5241,7 +5241,7 @@
     </row>
     <row r="185" spans="1:8">
       <c r="A185">
-        <v>1713819600</v>
+        <v>1713808800</v>
       </c>
       <c r="B185" t="s">
         <v>194</v>
@@ -5261,7 +5261,7 @@
     </row>
     <row r="186" spans="1:8">
       <c r="A186">
-        <v>1713823200</v>
+        <v>1713812400</v>
       </c>
       <c r="B186" t="s">
         <v>195</v>
@@ -5281,7 +5281,7 @@
     </row>
     <row r="187" spans="1:8">
       <c r="A187">
-        <v>1713826800</v>
+        <v>1713816000</v>
       </c>
       <c r="B187" t="s">
         <v>196</v>
@@ -5301,7 +5301,7 @@
     </row>
     <row r="188" spans="1:8">
       <c r="A188">
-        <v>1713830400</v>
+        <v>1713819600</v>
       </c>
       <c r="B188" t="s">
         <v>197</v>
@@ -5321,7 +5321,7 @@
     </row>
     <row r="189" spans="1:8">
       <c r="A189">
-        <v>1713834000</v>
+        <v>1713823200</v>
       </c>
       <c r="B189" t="s">
         <v>198</v>
@@ -5341,7 +5341,7 @@
     </row>
     <row r="190" spans="1:8">
       <c r="A190">
-        <v>1713837600</v>
+        <v>1713826800</v>
       </c>
       <c r="B190" t="s">
         <v>199</v>
@@ -5361,7 +5361,7 @@
     </row>
     <row r="191" spans="1:8">
       <c r="A191">
-        <v>1713841200</v>
+        <v>1713830400</v>
       </c>
       <c r="B191" t="s">
         <v>200</v>
@@ -5381,7 +5381,7 @@
     </row>
     <row r="192" spans="1:8">
       <c r="A192">
-        <v>1713844800</v>
+        <v>1713834000</v>
       </c>
       <c r="B192" t="s">
         <v>201</v>
@@ -5401,7 +5401,7 @@
     </row>
     <row r="193" spans="1:8">
       <c r="A193">
-        <v>1713848400</v>
+        <v>1713837600</v>
       </c>
       <c r="B193" t="s">
         <v>202</v>
@@ -5421,7 +5421,7 @@
     </row>
     <row r="194" spans="1:8">
       <c r="A194">
-        <v>1713852000</v>
+        <v>1713841200</v>
       </c>
       <c r="B194" t="s">
         <v>203</v>
@@ -5441,7 +5441,7 @@
     </row>
     <row r="195" spans="1:8">
       <c r="A195">
-        <v>1713855600</v>
+        <v>1713844800</v>
       </c>
       <c r="B195" t="s">
         <v>204</v>
@@ -5461,7 +5461,7 @@
     </row>
     <row r="196" spans="1:8">
       <c r="A196">
-        <v>1713859200</v>
+        <v>1713848400</v>
       </c>
       <c r="B196" t="s">
         <v>205</v>
@@ -5481,7 +5481,7 @@
     </row>
     <row r="197" spans="1:8">
       <c r="A197">
-        <v>1713862800</v>
+        <v>1713852000</v>
       </c>
       <c r="B197" t="s">
         <v>206</v>
@@ -5501,7 +5501,7 @@
     </row>
     <row r="198" spans="1:8">
       <c r="A198">
-        <v>1713866400</v>
+        <v>1713855600</v>
       </c>
       <c r="B198" t="s">
         <v>207</v>
@@ -5521,7 +5521,7 @@
     </row>
     <row r="199" spans="1:8">
       <c r="A199">
-        <v>1713870000</v>
+        <v>1713859200</v>
       </c>
       <c r="B199" t="s">
         <v>208</v>
@@ -5541,7 +5541,7 @@
     </row>
     <row r="200" spans="1:8">
       <c r="A200">
-        <v>1713873600</v>
+        <v>1713862800</v>
       </c>
       <c r="B200" t="s">
         <v>209</v>
@@ -5561,7 +5561,7 @@
     </row>
     <row r="201" spans="1:8">
       <c r="A201">
-        <v>1713877200</v>
+        <v>1713866400</v>
       </c>
       <c r="B201" t="s">
         <v>210</v>
@@ -5581,7 +5581,7 @@
     </row>
     <row r="202" spans="1:8">
       <c r="A202">
-        <v>1713880800</v>
+        <v>1713870000</v>
       </c>
       <c r="B202" t="s">
         <v>211</v>
@@ -5601,7 +5601,7 @@
     </row>
     <row r="203" spans="1:8">
       <c r="A203">
-        <v>1713884400</v>
+        <v>1713873600</v>
       </c>
       <c r="B203" t="s">
         <v>212</v>
@@ -5621,7 +5621,7 @@
     </row>
     <row r="204" spans="1:8">
       <c r="A204">
-        <v>1713888000</v>
+        <v>1713877200</v>
       </c>
       <c r="B204" t="s">
         <v>213</v>
@@ -5641,7 +5641,7 @@
     </row>
     <row r="205" spans="1:8">
       <c r="A205">
-        <v>1713891600</v>
+        <v>1713880800</v>
       </c>
       <c r="B205" t="s">
         <v>214</v>
@@ -5661,7 +5661,7 @@
     </row>
     <row r="206" spans="1:8">
       <c r="A206">
-        <v>1713895200</v>
+        <v>1713884400</v>
       </c>
       <c r="B206" t="s">
         <v>215</v>
@@ -5681,7 +5681,7 @@
     </row>
     <row r="207" spans="1:8">
       <c r="A207">
-        <v>1713898800</v>
+        <v>1713888000</v>
       </c>
       <c r="B207" t="s">
         <v>216</v>
@@ -5701,7 +5701,7 @@
     </row>
     <row r="208" spans="1:8">
       <c r="A208">
-        <v>1713902400</v>
+        <v>1713891600</v>
       </c>
       <c r="B208" t="s">
         <v>217</v>
@@ -5721,7 +5721,7 @@
     </row>
     <row r="209" spans="1:8">
       <c r="A209">
-        <v>1713906000</v>
+        <v>1713895200</v>
       </c>
       <c r="B209" t="s">
         <v>218</v>
@@ -5741,7 +5741,7 @@
     </row>
     <row r="210" spans="1:8">
       <c r="A210">
-        <v>1713909600</v>
+        <v>1713898800</v>
       </c>
       <c r="B210" t="s">
         <v>219</v>
@@ -5761,7 +5761,7 @@
     </row>
     <row r="211" spans="1:8">
       <c r="A211">
-        <v>1713913200</v>
+        <v>1713902400</v>
       </c>
       <c r="B211" t="s">
         <v>220</v>
@@ -5781,7 +5781,7 @@
     </row>
     <row r="212" spans="1:8">
       <c r="A212">
-        <v>1713916800</v>
+        <v>1713906000</v>
       </c>
       <c r="B212" t="s">
         <v>221</v>
@@ -5801,7 +5801,7 @@
     </row>
     <row r="213" spans="1:8">
       <c r="A213">
-        <v>1713920400</v>
+        <v>1713909600</v>
       </c>
       <c r="B213" t="s">
         <v>222</v>
@@ -5821,7 +5821,7 @@
     </row>
     <row r="214" spans="1:8">
       <c r="A214">
-        <v>1713924000</v>
+        <v>1713913200</v>
       </c>
       <c r="B214" t="s">
         <v>223</v>
@@ -5841,7 +5841,7 @@
     </row>
     <row r="215" spans="1:8">
       <c r="A215">
-        <v>1713927600</v>
+        <v>1713916800</v>
       </c>
       <c r="B215" t="s">
         <v>224</v>
@@ -5861,7 +5861,7 @@
     </row>
     <row r="216" spans="1:8">
       <c r="A216">
-        <v>1713931200</v>
+        <v>1713920400</v>
       </c>
       <c r="B216" t="s">
         <v>225</v>
@@ -5881,7 +5881,7 @@
     </row>
     <row r="217" spans="1:8">
       <c r="A217">
-        <v>1713934800</v>
+        <v>1713924000</v>
       </c>
       <c r="B217" t="s">
         <v>226</v>
@@ -5901,7 +5901,7 @@
     </row>
     <row r="218" spans="1:8">
       <c r="A218">
-        <v>1713938400</v>
+        <v>1713927600</v>
       </c>
       <c r="B218" t="s">
         <v>227</v>
@@ -5921,7 +5921,7 @@
     </row>
     <row r="219" spans="1:8">
       <c r="A219">
-        <v>1713942000</v>
+        <v>1713931200</v>
       </c>
       <c r="B219" t="s">
         <v>228</v>
@@ -5941,7 +5941,7 @@
     </row>
     <row r="220" spans="1:8">
       <c r="A220">
-        <v>1713945600</v>
+        <v>1713934800</v>
       </c>
       <c r="B220" t="s">
         <v>229</v>
@@ -5961,7 +5961,7 @@
     </row>
     <row r="221" spans="1:8">
       <c r="A221">
-        <v>1713949200</v>
+        <v>1713938400</v>
       </c>
       <c r="B221" t="s">
         <v>230</v>
@@ -5981,7 +5981,7 @@
     </row>
     <row r="222" spans="1:8">
       <c r="A222">
-        <v>1713952800</v>
+        <v>1713942000</v>
       </c>
       <c r="B222" t="s">
         <v>231</v>
@@ -6001,7 +6001,7 @@
     </row>
     <row r="223" spans="1:8">
       <c r="A223">
-        <v>1713956400</v>
+        <v>1713945600</v>
       </c>
       <c r="B223" t="s">
         <v>232</v>
@@ -6021,7 +6021,7 @@
     </row>
     <row r="224" spans="1:8">
       <c r="A224">
-        <v>1713960000</v>
+        <v>1713949200</v>
       </c>
       <c r="B224" t="s">
         <v>233</v>
@@ -6041,7 +6041,7 @@
     </row>
     <row r="225" spans="1:11">
       <c r="A225">
-        <v>1713963600</v>
+        <v>1713952800</v>
       </c>
       <c r="B225" t="s">
         <v>234</v>
@@ -6061,7 +6061,7 @@
     </row>
     <row r="226" spans="1:11">
       <c r="A226">
-        <v>1713967200</v>
+        <v>1713956400</v>
       </c>
       <c r="B226" t="s">
         <v>235</v>
@@ -6081,7 +6081,7 @@
     </row>
     <row r="227" spans="1:11">
       <c r="A227">
-        <v>1713970800</v>
+        <v>1713960000</v>
       </c>
       <c r="B227" t="s">
         <v>236</v>
@@ -6101,7 +6101,7 @@
     </row>
     <row r="228" spans="1:11">
       <c r="A228">
-        <v>1713974400</v>
+        <v>1713963600</v>
       </c>
       <c r="B228" t="s">
         <v>237</v>
@@ -6121,7 +6121,7 @@
     </row>
     <row r="229" spans="1:11">
       <c r="A229">
-        <v>1713978000</v>
+        <v>1713967200</v>
       </c>
       <c r="B229" t="s">
         <v>238</v>
@@ -6141,7 +6141,7 @@
     </row>
     <row r="230" spans="1:11">
       <c r="A230">
-        <v>1713981600</v>
+        <v>1713970800</v>
       </c>
       <c r="B230" t="s">
         <v>239</v>
@@ -6161,7 +6161,7 @@
     </row>
     <row r="231" spans="1:11">
       <c r="A231">
-        <v>1713985200</v>
+        <v>1713974400</v>
       </c>
       <c r="B231" t="s">
         <v>240</v>
@@ -6181,7 +6181,7 @@
     </row>
     <row r="232" spans="1:11">
       <c r="A232">
-        <v>1713988800</v>
+        <v>1713978000</v>
       </c>
       <c r="B232" t="s">
         <v>241</v>
@@ -6207,7 +6207,7 @@
     </row>
     <row r="233" spans="1:11">
       <c r="A233">
-        <v>1713992400</v>
+        <v>1713981600</v>
       </c>
       <c r="B233" t="s">
         <v>242</v>
@@ -6233,7 +6233,7 @@
     </row>
     <row r="234" spans="1:11">
       <c r="A234">
-        <v>1713996000</v>
+        <v>1713985200</v>
       </c>
       <c r="B234" t="s">
         <v>243</v>
@@ -6259,7 +6259,7 @@
     </row>
     <row r="235" spans="1:11">
       <c r="A235">
-        <v>1713999600</v>
+        <v>1713988800</v>
       </c>
       <c r="B235" t="s">
         <v>244</v>
@@ -6285,7 +6285,7 @@
     </row>
     <row r="236" spans="1:11">
       <c r="A236">
-        <v>1714003200</v>
+        <v>1713992400</v>
       </c>
       <c r="B236" t="s">
         <v>245</v>
@@ -6311,7 +6311,7 @@
     </row>
     <row r="237" spans="1:11">
       <c r="A237">
-        <v>1714006800</v>
+        <v>1713996000</v>
       </c>
       <c r="B237" t="s">
         <v>246</v>
@@ -6337,7 +6337,7 @@
     </row>
     <row r="238" spans="1:11">
       <c r="A238">
-        <v>1714010400</v>
+        <v>1713999600</v>
       </c>
       <c r="B238" t="s">
         <v>247</v>
@@ -6363,7 +6363,7 @@
     </row>
     <row r="239" spans="1:11">
       <c r="A239">
-        <v>1714014000</v>
+        <v>1714003200</v>
       </c>
       <c r="B239" t="s">
         <v>248</v>
@@ -6389,7 +6389,7 @@
     </row>
     <row r="240" spans="1:11">
       <c r="A240">
-        <v>1714017600</v>
+        <v>1714006800</v>
       </c>
       <c r="B240" t="s">
         <v>249</v>
@@ -6415,7 +6415,7 @@
     </row>
     <row r="241" spans="1:11">
       <c r="A241">
-        <v>1714021200</v>
+        <v>1714010400</v>
       </c>
       <c r="B241" t="s">
         <v>250</v>
@@ -6441,7 +6441,7 @@
     </row>
     <row r="242" spans="1:11">
       <c r="A242">
-        <v>1714024800</v>
+        <v>1714014000</v>
       </c>
       <c r="B242" t="s">
         <v>251</v>
@@ -6467,7 +6467,7 @@
     </row>
     <row r="243" spans="1:11">
       <c r="A243">
-        <v>1714028400</v>
+        <v>1714017600</v>
       </c>
       <c r="B243" t="s">
         <v>252</v>
@@ -6493,7 +6493,7 @@
     </row>
     <row r="244" spans="1:11">
       <c r="A244">
-        <v>1714032000</v>
+        <v>1714021200</v>
       </c>
       <c r="B244" t="s">
         <v>253</v>
@@ -6519,7 +6519,7 @@
     </row>
     <row r="245" spans="1:11">
       <c r="A245">
-        <v>1714035600</v>
+        <v>1714024800</v>
       </c>
       <c r="B245" t="s">
         <v>254</v>
@@ -6545,7 +6545,7 @@
     </row>
     <row r="246" spans="1:11">
       <c r="A246">
-        <v>1714039200</v>
+        <v>1714028400</v>
       </c>
       <c r="B246" t="s">
         <v>255</v>
@@ -6571,7 +6571,7 @@
     </row>
     <row r="247" spans="1:11">
       <c r="A247">
-        <v>1714042800</v>
+        <v>1714032000</v>
       </c>
       <c r="B247" t="s">
         <v>256</v>
@@ -6597,7 +6597,7 @@
     </row>
     <row r="248" spans="1:11">
       <c r="A248">
-        <v>1714046400</v>
+        <v>1714035600</v>
       </c>
       <c r="B248" t="s">
         <v>257</v>
@@ -6623,7 +6623,7 @@
     </row>
     <row r="249" spans="1:11">
       <c r="A249">
-        <v>1714050000</v>
+        <v>1714039200</v>
       </c>
       <c r="B249" t="s">
         <v>258</v>
@@ -6649,7 +6649,7 @@
     </row>
     <row r="250" spans="1:11">
       <c r="A250">
-        <v>1714053600</v>
+        <v>1714042800</v>
       </c>
       <c r="B250" t="s">
         <v>259</v>
@@ -6675,7 +6675,7 @@
     </row>
     <row r="251" spans="1:11">
       <c r="A251">
-        <v>1714057200</v>
+        <v>1714046400</v>
       </c>
       <c r="B251" t="s">
         <v>260</v>
@@ -6701,7 +6701,7 @@
     </row>
     <row r="252" spans="1:11">
       <c r="A252">
-        <v>1714060800</v>
+        <v>1714050000</v>
       </c>
       <c r="B252" t="s">
         <v>261</v>
@@ -6727,7 +6727,7 @@
     </row>
     <row r="253" spans="1:11">
       <c r="A253">
-        <v>1714064400</v>
+        <v>1714053600</v>
       </c>
       <c r="B253" t="s">
         <v>262</v>
@@ -6753,7 +6753,7 @@
     </row>
     <row r="254" spans="1:11">
       <c r="A254">
-        <v>1714068000</v>
+        <v>1714057200</v>
       </c>
       <c r="B254" t="s">
         <v>263</v>
@@ -6779,7 +6779,7 @@
     </row>
     <row r="255" spans="1:11">
       <c r="A255">
-        <v>1714071600</v>
+        <v>1714060800</v>
       </c>
       <c r="B255" t="s">
         <v>264</v>
@@ -6805,7 +6805,7 @@
     </row>
     <row r="256" spans="1:11">
       <c r="A256">
-        <v>1714075200</v>
+        <v>1714064400</v>
       </c>
       <c r="B256" t="s">
         <v>265</v>
@@ -6831,7 +6831,7 @@
     </row>
     <row r="257" spans="1:11">
       <c r="A257">
-        <v>1714078800</v>
+        <v>1714068000</v>
       </c>
       <c r="B257" t="s">
         <v>266</v>
@@ -6857,7 +6857,7 @@
     </row>
     <row r="258" spans="1:11">
       <c r="A258">
-        <v>1714082400</v>
+        <v>1714071600</v>
       </c>
       <c r="B258" t="s">
         <v>267</v>
@@ -6883,7 +6883,7 @@
     </row>
     <row r="259" spans="1:11">
       <c r="A259">
-        <v>1714086000</v>
+        <v>1714075200</v>
       </c>
       <c r="B259" t="s">
         <v>268</v>
@@ -6909,7 +6909,7 @@
     </row>
     <row r="260" spans="1:11">
       <c r="A260">
-        <v>1714089600</v>
+        <v>1714078800</v>
       </c>
       <c r="B260" t="s">
         <v>269</v>
@@ -6935,7 +6935,7 @@
     </row>
     <row r="261" spans="1:11">
       <c r="A261">
-        <v>1714093200</v>
+        <v>1714082400</v>
       </c>
       <c r="B261" t="s">
         <v>270</v>
@@ -6961,7 +6961,7 @@
     </row>
     <row r="262" spans="1:11">
       <c r="A262">
-        <v>1714096800</v>
+        <v>1714086000</v>
       </c>
       <c r="B262" t="s">
         <v>271</v>
@@ -6987,7 +6987,7 @@
     </row>
     <row r="263" spans="1:11">
       <c r="A263">
-        <v>1714100400</v>
+        <v>1714089600</v>
       </c>
       <c r="B263" t="s">
         <v>272</v>
@@ -7013,7 +7013,7 @@
     </row>
     <row r="264" spans="1:11">
       <c r="A264">
-        <v>1714104000</v>
+        <v>1714093200</v>
       </c>
       <c r="B264" t="s">
         <v>273</v>
@@ -7039,7 +7039,7 @@
     </row>
     <row r="265" spans="1:11">
       <c r="A265">
-        <v>1714107600</v>
+        <v>1714096800</v>
       </c>
       <c r="B265" t="s">
         <v>274</v>
@@ -7065,7 +7065,7 @@
     </row>
     <row r="266" spans="1:11">
       <c r="A266">
-        <v>1714111200</v>
+        <v>1714100400</v>
       </c>
       <c r="B266" t="s">
         <v>275</v>
@@ -7091,7 +7091,7 @@
     </row>
     <row r="267" spans="1:11">
       <c r="A267">
-        <v>1714114800</v>
+        <v>1714104000</v>
       </c>
       <c r="B267" t="s">
         <v>276</v>
@@ -7117,7 +7117,7 @@
     </row>
     <row r="268" spans="1:11">
       <c r="A268">
-        <v>1714118400</v>
+        <v>1714107600</v>
       </c>
       <c r="B268" t="s">
         <v>277</v>
@@ -7143,7 +7143,7 @@
     </row>
     <row r="269" spans="1:11">
       <c r="A269">
-        <v>1714122000</v>
+        <v>1714111200</v>
       </c>
       <c r="B269" t="s">
         <v>278</v>
@@ -7169,7 +7169,7 @@
     </row>
     <row r="270" spans="1:11">
       <c r="A270">
-        <v>1714125600</v>
+        <v>1714114800</v>
       </c>
       <c r="B270" t="s">
         <v>279</v>
@@ -7195,7 +7195,7 @@
     </row>
     <row r="271" spans="1:11">
       <c r="A271">
-        <v>1714129200</v>
+        <v>1714118400</v>
       </c>
       <c r="B271" t="s">
         <v>280</v>
@@ -7221,7 +7221,7 @@
     </row>
     <row r="272" spans="1:11">
       <c r="A272">
-        <v>1714132800</v>
+        <v>1714122000</v>
       </c>
       <c r="B272" t="s">
         <v>281</v>
@@ -7247,7 +7247,7 @@
     </row>
     <row r="273" spans="1:11">
       <c r="A273">
-        <v>1714136400</v>
+        <v>1714125600</v>
       </c>
       <c r="B273" t="s">
         <v>282</v>
@@ -7273,7 +7273,7 @@
     </row>
     <row r="274" spans="1:11">
       <c r="A274">
-        <v>1714140000</v>
+        <v>1714129200</v>
       </c>
       <c r="B274" t="s">
         <v>283</v>
@@ -7299,7 +7299,7 @@
     </row>
     <row r="275" spans="1:11">
       <c r="A275">
-        <v>1714143600</v>
+        <v>1714132800</v>
       </c>
       <c r="B275" t="s">
         <v>284</v>
@@ -7325,7 +7325,7 @@
     </row>
     <row r="276" spans="1:11">
       <c r="A276">
-        <v>1714147200</v>
+        <v>1714136400</v>
       </c>
       <c r="B276" t="s">
         <v>285</v>
@@ -7351,7 +7351,7 @@
     </row>
     <row r="277" spans="1:11">
       <c r="A277">
-        <v>1714150800</v>
+        <v>1714140000</v>
       </c>
       <c r="B277" t="s">
         <v>286</v>
@@ -7377,7 +7377,7 @@
     </row>
     <row r="278" spans="1:11">
       <c r="A278">
-        <v>1714154400</v>
+        <v>1714143600</v>
       </c>
       <c r="B278" t="s">
         <v>287</v>
@@ -7403,7 +7403,7 @@
     </row>
     <row r="279" spans="1:11">
       <c r="A279">
-        <v>1714158000</v>
+        <v>1714147200</v>
       </c>
       <c r="B279" t="s">
         <v>288</v>
@@ -7429,7 +7429,7 @@
     </row>
     <row r="280" spans="1:11">
       <c r="A280">
-        <v>1714161600</v>
+        <v>1714150800</v>
       </c>
       <c r="B280" t="s">
         <v>289</v>
@@ -7455,7 +7455,7 @@
     </row>
     <row r="281" spans="1:11">
       <c r="A281">
-        <v>1714165200</v>
+        <v>1714154400</v>
       </c>
       <c r="B281" t="s">
         <v>290</v>
@@ -7481,7 +7481,7 @@
     </row>
     <row r="282" spans="1:11">
       <c r="A282">
-        <v>1714168800</v>
+        <v>1714158000</v>
       </c>
       <c r="B282" t="s">
         <v>291</v>
@@ -7507,7 +7507,7 @@
     </row>
     <row r="283" spans="1:11">
       <c r="A283">
-        <v>1714172400</v>
+        <v>1714161600</v>
       </c>
       <c r="B283" t="s">
         <v>292</v>
@@ -7533,7 +7533,7 @@
     </row>
     <row r="284" spans="1:11">
       <c r="A284">
-        <v>1714176000</v>
+        <v>1714165200</v>
       </c>
       <c r="B284" t="s">
         <v>293</v>
@@ -7559,7 +7559,7 @@
     </row>
     <row r="285" spans="1:11">
       <c r="A285">
-        <v>1714179600</v>
+        <v>1714168800</v>
       </c>
       <c r="B285" t="s">
         <v>294</v>
@@ -7585,7 +7585,7 @@
     </row>
     <row r="286" spans="1:11">
       <c r="A286">
-        <v>1714183200</v>
+        <v>1714172400</v>
       </c>
       <c r="B286" t="s">
         <v>295</v>
@@ -7611,7 +7611,7 @@
     </row>
     <row r="287" spans="1:11">
       <c r="A287">
-        <v>1714186800</v>
+        <v>1714176000</v>
       </c>
       <c r="B287" t="s">
         <v>296</v>
@@ -7637,7 +7637,7 @@
     </row>
     <row r="288" spans="1:11">
       <c r="A288">
-        <v>1714190400</v>
+        <v>1714179600</v>
       </c>
       <c r="B288" t="s">
         <v>297</v>
@@ -7663,7 +7663,7 @@
     </row>
     <row r="289" spans="1:11">
       <c r="A289">
-        <v>1714194000</v>
+        <v>1714183200</v>
       </c>
       <c r="B289" t="s">
         <v>298</v>
@@ -7689,7 +7689,7 @@
     </row>
     <row r="290" spans="1:11">
       <c r="A290">
-        <v>1714197600</v>
+        <v>1714186800</v>
       </c>
       <c r="B290" t="s">
         <v>299</v>
@@ -7715,7 +7715,7 @@
     </row>
     <row r="291" spans="1:11">
       <c r="A291">
-        <v>1714201200</v>
+        <v>1714190400</v>
       </c>
       <c r="B291" t="s">
         <v>300</v>
@@ -7741,7 +7741,7 @@
     </row>
     <row r="292" spans="1:11">
       <c r="A292">
-        <v>1714204800</v>
+        <v>1714194000</v>
       </c>
       <c r="B292" t="s">
         <v>301</v>
@@ -7767,7 +7767,7 @@
     </row>
     <row r="293" spans="1:11">
       <c r="A293">
-        <v>1714208400</v>
+        <v>1714197600</v>
       </c>
       <c r="B293" t="s">
         <v>302</v>
@@ -7793,7 +7793,7 @@
     </row>
     <row r="294" spans="1:11">
       <c r="A294">
-        <v>1714212000</v>
+        <v>1714201200</v>
       </c>
       <c r="B294" t="s">
         <v>303</v>
@@ -7819,7 +7819,7 @@
     </row>
     <row r="295" spans="1:11">
       <c r="A295">
-        <v>1714215600</v>
+        <v>1714204800</v>
       </c>
       <c r="B295" t="s">
         <v>304</v>
@@ -7845,7 +7845,7 @@
     </row>
     <row r="296" spans="1:11">
       <c r="A296">
-        <v>1714219200</v>
+        <v>1714208400</v>
       </c>
       <c r="B296" t="s">
         <v>305</v>
@@ -7871,7 +7871,7 @@
     </row>
     <row r="297" spans="1:11">
       <c r="A297">
-        <v>1714222800</v>
+        <v>1714212000</v>
       </c>
       <c r="B297" t="s">
         <v>306</v>
@@ -7897,7 +7897,7 @@
     </row>
     <row r="298" spans="1:11">
       <c r="A298">
-        <v>1714226400</v>
+        <v>1714215600</v>
       </c>
       <c r="B298" t="s">
         <v>307</v>
@@ -7923,7 +7923,7 @@
     </row>
     <row r="299" spans="1:11">
       <c r="A299">
-        <v>1714230000</v>
+        <v>1714219200</v>
       </c>
       <c r="B299" t="s">
         <v>308</v>
@@ -7949,7 +7949,7 @@
     </row>
     <row r="300" spans="1:11">
       <c r="A300">
-        <v>1714233600</v>
+        <v>1714222800</v>
       </c>
       <c r="B300" t="s">
         <v>309</v>
@@ -7975,7 +7975,7 @@
     </row>
     <row r="301" spans="1:11">
       <c r="A301">
-        <v>1714237200</v>
+        <v>1714226400</v>
       </c>
       <c r="B301" t="s">
         <v>310</v>
@@ -8001,7 +8001,7 @@
     </row>
     <row r="302" spans="1:11">
       <c r="A302">
-        <v>1714240800</v>
+        <v>1714230000</v>
       </c>
       <c r="B302" t="s">
         <v>311</v>
@@ -8027,7 +8027,7 @@
     </row>
     <row r="303" spans="1:11">
       <c r="A303">
-        <v>1714244400</v>
+        <v>1714233600</v>
       </c>
       <c r="B303" t="s">
         <v>312</v>
@@ -8053,7 +8053,7 @@
     </row>
     <row r="304" spans="1:11">
       <c r="A304">
-        <v>1714248000</v>
+        <v>1714237200</v>
       </c>
       <c r="B304" t="s">
         <v>313</v>
@@ -8079,7 +8079,7 @@
     </row>
     <row r="305" spans="1:11">
       <c r="A305">
-        <v>1714251600</v>
+        <v>1714240800</v>
       </c>
       <c r="B305" t="s">
         <v>314</v>
@@ -8105,7 +8105,7 @@
     </row>
     <row r="306" spans="1:11">
       <c r="A306">
-        <v>1714255200</v>
+        <v>1714244400</v>
       </c>
       <c r="B306" t="s">
         <v>315</v>
@@ -8131,7 +8131,7 @@
     </row>
     <row r="307" spans="1:11">
       <c r="A307">
-        <v>1714258800</v>
+        <v>1714248000</v>
       </c>
       <c r="B307" t="s">
         <v>316</v>
@@ -8157,7 +8157,7 @@
     </row>
     <row r="308" spans="1:11">
       <c r="A308">
-        <v>1714262400</v>
+        <v>1714251600</v>
       </c>
       <c r="B308" t="s">
         <v>317</v>
@@ -8183,7 +8183,7 @@
     </row>
     <row r="309" spans="1:11">
       <c r="A309">
-        <v>1714266000</v>
+        <v>1714255200</v>
       </c>
       <c r="B309" t="s">
         <v>318</v>
@@ -8209,7 +8209,7 @@
     </row>
     <row r="310" spans="1:11">
       <c r="A310">
-        <v>1714269600</v>
+        <v>1714258800</v>
       </c>
       <c r="B310" t="s">
         <v>319</v>
@@ -8235,7 +8235,7 @@
     </row>
     <row r="311" spans="1:11">
       <c r="A311">
-        <v>1714273200</v>
+        <v>1714262400</v>
       </c>
       <c r="B311" t="s">
         <v>320</v>
@@ -8261,7 +8261,7 @@
     </row>
     <row r="312" spans="1:11">
       <c r="A312">
-        <v>1714276800</v>
+        <v>1714266000</v>
       </c>
       <c r="B312" t="s">
         <v>321</v>
@@ -8287,7 +8287,7 @@
     </row>
     <row r="313" spans="1:11">
       <c r="A313">
-        <v>1714280400</v>
+        <v>1714269600</v>
       </c>
       <c r="B313" t="s">
         <v>322</v>
@@ -8313,7 +8313,7 @@
     </row>
     <row r="314" spans="1:11">
       <c r="A314">
-        <v>1714284000</v>
+        <v>1714273200</v>
       </c>
       <c r="B314" t="s">
         <v>323</v>
@@ -8339,7 +8339,7 @@
     </row>
     <row r="315" spans="1:11">
       <c r="A315">
-        <v>1714287600</v>
+        <v>1714276800</v>
       </c>
       <c r="B315" t="s">
         <v>324</v>
@@ -8365,7 +8365,7 @@
     </row>
     <row r="316" spans="1:11">
       <c r="A316">
-        <v>1714291200</v>
+        <v>1714280400</v>
       </c>
       <c r="B316" t="s">
         <v>325</v>
@@ -8391,7 +8391,7 @@
     </row>
     <row r="317" spans="1:11">
       <c r="A317">
-        <v>1714294800</v>
+        <v>1714284000</v>
       </c>
       <c r="B317" t="s">
         <v>326</v>
@@ -8417,7 +8417,7 @@
     </row>
     <row r="318" spans="1:11">
       <c r="A318">
-        <v>1714298400</v>
+        <v>1714287600</v>
       </c>
       <c r="B318" t="s">
         <v>327</v>
@@ -8443,7 +8443,7 @@
     </row>
     <row r="319" spans="1:11">
       <c r="A319">
-        <v>1714302000</v>
+        <v>1714291200</v>
       </c>
       <c r="B319" t="s">
         <v>328</v>
@@ -8469,7 +8469,7 @@
     </row>
     <row r="320" spans="1:11">
       <c r="A320">
-        <v>1714305600</v>
+        <v>1714294800</v>
       </c>
       <c r="B320" t="s">
         <v>329</v>
@@ -8495,7 +8495,7 @@
     </row>
     <row r="321" spans="1:11">
       <c r="A321">
-        <v>1714309200</v>
+        <v>1714298400</v>
       </c>
       <c r="B321" t="s">
         <v>330</v>
@@ -8521,7 +8521,7 @@
     </row>
     <row r="322" spans="1:11">
       <c r="A322">
-        <v>1714312800</v>
+        <v>1714302000</v>
       </c>
       <c r="B322" t="s">
         <v>331</v>
@@ -8547,7 +8547,7 @@
     </row>
     <row r="323" spans="1:11">
       <c r="A323">
-        <v>1714316400</v>
+        <v>1714305600</v>
       </c>
       <c r="B323" t="s">
         <v>332</v>
@@ -8573,7 +8573,7 @@
     </row>
     <row r="324" spans="1:11">
       <c r="A324">
-        <v>1714320000</v>
+        <v>1714309200</v>
       </c>
       <c r="B324" t="s">
         <v>333</v>
@@ -8599,7 +8599,7 @@
     </row>
     <row r="325" spans="1:11">
       <c r="A325">
-        <v>1714323600</v>
+        <v>1714312800</v>
       </c>
       <c r="B325" t="s">
         <v>334</v>
@@ -8625,7 +8625,7 @@
     </row>
     <row r="326" spans="1:11">
       <c r="A326">
-        <v>1714327200</v>
+        <v>1714316400</v>
       </c>
       <c r="B326" t="s">
         <v>335</v>
@@ -8651,7 +8651,7 @@
     </row>
     <row r="327" spans="1:11">
       <c r="A327">
-        <v>1714330800</v>
+        <v>1714320000</v>
       </c>
       <c r="B327" t="s">
         <v>336</v>
@@ -8677,7 +8677,7 @@
     </row>
     <row r="328" spans="1:11">
       <c r="A328">
-        <v>1714334400</v>
+        <v>1714323600</v>
       </c>
       <c r="B328" t="s">
         <v>337</v>
@@ -8703,7 +8703,7 @@
     </row>
     <row r="329" spans="1:11">
       <c r="A329">
-        <v>1714338000</v>
+        <v>1714327200</v>
       </c>
       <c r="B329" t="s">
         <v>338</v>
@@ -8729,7 +8729,7 @@
     </row>
     <row r="330" spans="1:11">
       <c r="A330">
-        <v>1714341600</v>
+        <v>1714330800</v>
       </c>
       <c r="B330" t="s">
         <v>339</v>
@@ -8755,7 +8755,7 @@
     </row>
     <row r="331" spans="1:11">
       <c r="A331">
-        <v>1714345200</v>
+        <v>1714334400</v>
       </c>
       <c r="B331" t="s">
         <v>340</v>
@@ -8781,7 +8781,7 @@
     </row>
     <row r="332" spans="1:11">
       <c r="A332">
-        <v>1714348800</v>
+        <v>1714338000</v>
       </c>
       <c r="B332" t="s">
         <v>341</v>
@@ -8807,7 +8807,7 @@
     </row>
     <row r="333" spans="1:11">
       <c r="A333">
-        <v>1714352400</v>
+        <v>1714341600</v>
       </c>
       <c r="B333" t="s">
         <v>342</v>
@@ -8833,7 +8833,7 @@
     </row>
     <row r="334" spans="1:11">
       <c r="A334">
-        <v>1714356000</v>
+        <v>1714345200</v>
       </c>
       <c r="B334" t="s">
         <v>343</v>
@@ -8859,7 +8859,7 @@
     </row>
     <row r="335" spans="1:11">
       <c r="A335">
-        <v>1714359600</v>
+        <v>1714348800</v>
       </c>
       <c r="B335" t="s">
         <v>344</v>
@@ -8885,7 +8885,7 @@
     </row>
     <row r="336" spans="1:11">
       <c r="A336">
-        <v>1714363200</v>
+        <v>1714352400</v>
       </c>
       <c r="B336" t="s">
         <v>345</v>
@@ -8911,7 +8911,7 @@
     </row>
     <row r="337" spans="1:11">
       <c r="A337">
-        <v>1714366800</v>
+        <v>1714356000</v>
       </c>
       <c r="B337" t="s">
         <v>346</v>
@@ -8937,7 +8937,7 @@
     </row>
     <row r="338" spans="1:11">
       <c r="A338">
-        <v>1714370400</v>
+        <v>1714359600</v>
       </c>
       <c r="B338" t="s">
         <v>347</v>
@@ -8963,7 +8963,7 @@
     </row>
     <row r="339" spans="1:11">
       <c r="A339">
-        <v>1714374000</v>
+        <v>1714363200</v>
       </c>
       <c r="B339" t="s">
         <v>348</v>
@@ -8989,7 +8989,7 @@
     </row>
     <row r="340" spans="1:11">
       <c r="A340">
-        <v>1714377600</v>
+        <v>1714366800</v>
       </c>
       <c r="B340" t="s">
         <v>349</v>
@@ -9015,7 +9015,7 @@
     </row>
     <row r="341" spans="1:11">
       <c r="A341">
-        <v>1714381200</v>
+        <v>1714370400</v>
       </c>
       <c r="B341" t="s">
         <v>350</v>
@@ -9041,7 +9041,7 @@
     </row>
     <row r="342" spans="1:11">
       <c r="A342">
-        <v>1714384800</v>
+        <v>1714374000</v>
       </c>
       <c r="B342" t="s">
         <v>351</v>
@@ -9067,7 +9067,7 @@
     </row>
     <row r="343" spans="1:11">
       <c r="A343">
-        <v>1714388400</v>
+        <v>1714377600</v>
       </c>
       <c r="B343" t="s">
         <v>352</v>
@@ -9093,7 +9093,7 @@
     </row>
     <row r="344" spans="1:11">
       <c r="A344">
-        <v>1714392000</v>
+        <v>1714381200</v>
       </c>
       <c r="B344" t="s">
         <v>353</v>
@@ -9119,7 +9119,7 @@
     </row>
     <row r="345" spans="1:11">
       <c r="A345">
-        <v>1714395600</v>
+        <v>1714384800</v>
       </c>
       <c r="B345" t="s">
         <v>354</v>
@@ -9145,7 +9145,7 @@
     </row>
     <row r="346" spans="1:11">
       <c r="A346">
-        <v>1714399200</v>
+        <v>1714388400</v>
       </c>
       <c r="B346" t="s">
         <v>355</v>
@@ -9171,7 +9171,7 @@
     </row>
     <row r="347" spans="1:11">
       <c r="A347">
-        <v>1714402800</v>
+        <v>1714392000</v>
       </c>
       <c r="B347" t="s">
         <v>356</v>
@@ -9197,7 +9197,7 @@
     </row>
     <row r="348" spans="1:11">
       <c r="A348">
-        <v>1714406400</v>
+        <v>1714395600</v>
       </c>
       <c r="B348" t="s">
         <v>357</v>
@@ -9223,7 +9223,7 @@
     </row>
     <row r="349" spans="1:11">
       <c r="A349">
-        <v>1714410000</v>
+        <v>1714399200</v>
       </c>
       <c r="B349" t="s">
         <v>358</v>
@@ -9249,7 +9249,7 @@
     </row>
     <row r="350" spans="1:11">
       <c r="A350">
-        <v>1714413600</v>
+        <v>1714402800</v>
       </c>
       <c r="B350" t="s">
         <v>359</v>
@@ -9275,7 +9275,7 @@
     </row>
     <row r="351" spans="1:11">
       <c r="A351">
-        <v>1714417200</v>
+        <v>1714406400</v>
       </c>
       <c r="B351" t="s">
         <v>360</v>
@@ -9301,7 +9301,7 @@
     </row>
     <row r="352" spans="1:11">
       <c r="A352">
-        <v>1714420800</v>
+        <v>1714410000</v>
       </c>
       <c r="B352" t="s">
         <v>361</v>
@@ -9327,7 +9327,7 @@
     </row>
     <row r="353" spans="1:11">
       <c r="A353">
-        <v>1714424400</v>
+        <v>1714413600</v>
       </c>
       <c r="B353" t="s">
         <v>362</v>
@@ -9353,7 +9353,7 @@
     </row>
     <row r="354" spans="1:11">
       <c r="A354">
-        <v>1714428000</v>
+        <v>1714417200</v>
       </c>
       <c r="B354" t="s">
         <v>363</v>
@@ -9379,7 +9379,7 @@
     </row>
     <row r="355" spans="1:11">
       <c r="A355">
-        <v>1714431600</v>
+        <v>1714420800</v>
       </c>
       <c r="B355" t="s">
         <v>364</v>
@@ -9405,7 +9405,7 @@
     </row>
     <row r="356" spans="1:11">
       <c r="A356">
-        <v>1714435200</v>
+        <v>1714424400</v>
       </c>
       <c r="B356" t="s">
         <v>365</v>
@@ -9431,7 +9431,7 @@
     </row>
     <row r="357" spans="1:11">
       <c r="A357">
-        <v>1714438800</v>
+        <v>1714428000</v>
       </c>
       <c r="B357" t="s">
         <v>366</v>
@@ -9457,7 +9457,7 @@
     </row>
     <row r="358" spans="1:11">
       <c r="A358">
-        <v>1714442400</v>
+        <v>1714431600</v>
       </c>
       <c r="B358" t="s">
         <v>367</v>
@@ -9483,7 +9483,7 @@
     </row>
     <row r="359" spans="1:11">
       <c r="A359">
-        <v>1714446000</v>
+        <v>1714435200</v>
       </c>
       <c r="B359" t="s">
         <v>368</v>
@@ -9509,7 +9509,7 @@
     </row>
     <row r="360" spans="1:11">
       <c r="A360">
-        <v>1714449600</v>
+        <v>1714438800</v>
       </c>
       <c r="B360" t="s">
         <v>369</v>
@@ -9535,7 +9535,7 @@
     </row>
     <row r="361" spans="1:11">
       <c r="A361">
-        <v>1714453200</v>
+        <v>1714442400</v>
       </c>
       <c r="B361" t="s">
         <v>370</v>
@@ -9561,7 +9561,7 @@
     </row>
     <row r="362" spans="1:11">
       <c r="A362">
-        <v>1714456800</v>
+        <v>1714446000</v>
       </c>
       <c r="B362" t="s">
         <v>371</v>
@@ -9587,7 +9587,7 @@
     </row>
     <row r="363" spans="1:11">
       <c r="A363">
-        <v>1714460400</v>
+        <v>1714449600</v>
       </c>
       <c r="B363" t="s">
         <v>372</v>
@@ -9613,7 +9613,7 @@
     </row>
     <row r="364" spans="1:11">
       <c r="A364">
-        <v>1714464000</v>
+        <v>1714453200</v>
       </c>
       <c r="B364" t="s">
         <v>373</v>
@@ -9639,7 +9639,7 @@
     </row>
     <row r="365" spans="1:11">
       <c r="A365">
-        <v>1714467600</v>
+        <v>1714456800</v>
       </c>
       <c r="B365" t="s">
         <v>374</v>
@@ -9665,7 +9665,7 @@
     </row>
     <row r="366" spans="1:11">
       <c r="A366">
-        <v>1714471200</v>
+        <v>1714460400</v>
       </c>
       <c r="B366" t="s">
         <v>375</v>
@@ -9691,7 +9691,7 @@
     </row>
     <row r="367" spans="1:11">
       <c r="A367">
-        <v>1714474800</v>
+        <v>1714464000</v>
       </c>
       <c r="B367" t="s">
         <v>376</v>
@@ -9717,7 +9717,7 @@
     </row>
     <row r="368" spans="1:11">
       <c r="A368">
-        <v>1714478400</v>
+        <v>1714467600</v>
       </c>
       <c r="B368" t="s">
         <v>377</v>
@@ -9743,7 +9743,7 @@
     </row>
     <row r="369" spans="1:11">
       <c r="A369">
-        <v>1714482000</v>
+        <v>1714471200</v>
       </c>
       <c r="B369" t="s">
         <v>378</v>
@@ -9769,7 +9769,7 @@
     </row>
     <row r="370" spans="1:11">
       <c r="A370">
-        <v>1714485600</v>
+        <v>1714474800</v>
       </c>
       <c r="B370" t="s">
         <v>379</v>
@@ -9795,7 +9795,7 @@
     </row>
     <row r="371" spans="1:11">
       <c r="A371">
-        <v>1714489200</v>
+        <v>1714478400</v>
       </c>
       <c r="B371" t="s">
         <v>380</v>
@@ -9821,7 +9821,7 @@
     </row>
     <row r="372" spans="1:11">
       <c r="A372">
-        <v>1714492800</v>
+        <v>1714482000</v>
       </c>
       <c r="B372" t="s">
         <v>381</v>
@@ -9847,7 +9847,7 @@
     </row>
     <row r="373" spans="1:11">
       <c r="A373">
-        <v>1714496400</v>
+        <v>1714485600</v>
       </c>
       <c r="B373" t="s">
         <v>382</v>
@@ -9873,7 +9873,7 @@
     </row>
     <row r="374" spans="1:11">
       <c r="A374">
-        <v>1714500000</v>
+        <v>1714489200</v>
       </c>
       <c r="B374" t="s">
         <v>383</v>
@@ -9899,7 +9899,7 @@
     </row>
     <row r="375" spans="1:11">
       <c r="A375">
-        <v>1714503600</v>
+        <v>1714492800</v>
       </c>
       <c r="B375" t="s">
         <v>384</v>
@@ -9925,7 +9925,7 @@
     </row>
     <row r="376" spans="1:11">
       <c r="A376">
-        <v>1714507200</v>
+        <v>1714496400</v>
       </c>
       <c r="B376" t="s">
         <v>385</v>
@@ -9951,7 +9951,7 @@
     </row>
     <row r="377" spans="1:11">
       <c r="A377">
-        <v>1714510800</v>
+        <v>1714500000</v>
       </c>
       <c r="B377" t="s">
         <v>386</v>
@@ -9977,7 +9977,7 @@
     </row>
     <row r="378" spans="1:11">
       <c r="A378">
-        <v>1714514400</v>
+        <v>1714503600</v>
       </c>
       <c r="B378" t="s">
         <v>387</v>
@@ -10003,7 +10003,7 @@
     </row>
     <row r="379" spans="1:11">
       <c r="A379">
-        <v>1714518000</v>
+        <v>1714507200</v>
       </c>
       <c r="B379" t="s">
         <v>388</v>

</xml_diff>